<commit_message>
fix:Bug fixed sorting and assets
</commit_message>
<xml_diff>
--- a/src/data_add/users.xlsx
+++ b/src/data_add/users.xlsx
@@ -52,7 +52,7 @@
     <t>Yuvabe</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"id":"YB-99-M ","type":"Monitor"},{"id":"YB-92-L","type":"Laptop"},{"id":"YB-92-MS","type":"Mouse"},{"id":"YB-39-H","type":"Headphone"}]
+    <t xml:space="preserve">[{"id":"YB-99 ","type":"Monitor"},{"id":"YB-92-L","type":"Laptop"},{"id":"YB-92","type":"Mouse"},{"id":"YB-39-H","type":"Headphone"}]
 </t>
   </si>
   <si>
@@ -68,7 +68,8 @@
     <t>hp@yuvabe.com</t>
   </si>
   <si>
-    <t>[{"id":"YB-100-M ","type":"Monitor"},{"id":"YB-93-L","type":"Laptop"},{"id":"YB-93-MS","type":"Mouse"},{"id":"YB-80-H","type":"Headphone"}]</t>
+    <t xml:space="preserve">[{"id":"YB-19 ","type":"Monitor"},{"id":"YB-19","type":"Laptop"},{"id":"YB-19","type":"Mouse"},{"id":"YB-19","type":"Headphone"}]
+</t>
   </si>
   <si>
     <t>Mentor</t>
@@ -80,7 +81,7 @@
     <t>hariharan@quilt.ai</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"id":"YB-11-M ","type":"Monitor"},{"id":"YB-11-L","type":"Laptop"},{"id":"YB-11-MS","type":"Mouse"},{"id":"YB-11-H","type":"Headphone"}]
+    <t xml:space="preserve">[{"id":"YB-92 ","type":"Monitor"},{"id":"YB-11-L","type":"Laptop"},{"id":"YB-11-MS","type":"Mouse"},{"id":"YB-11-H","type":"Headphone"}]
 </t>
   </si>
   <si>
@@ -170,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +183,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -232,8 +239,8 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -617,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="34.5">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>